<commit_message>
metrica 2 dati ok
</commit_message>
<xml_diff>
--- a/documentation/LagIncreaseDo/LagIncreaseDo.xlsx
+++ b/documentation/LagIncreaseDo/LagIncreaseDo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giacomoponzuoli/Desktop/unifi_phd/documentation/LagIncreaseDo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattiamarilli/Progetti/unifi_phd/documentation/LagIncreaseDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F683E9A1-F1E2-EA4F-8DDD-002B4B12F1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD65611-431C-F34E-91BA-8C29CEB5E99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15780" activeTab="3" xr2:uid="{9C1D837C-A722-4248-A86A-CE69ED4B7649}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15780" activeTab="1" xr2:uid="{9C1D837C-A722-4248-A86A-CE69ED4B7649}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="31">
   <si>
     <t>Insert professor</t>
   </si>
@@ -489,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DA2B74-2347-0347-86D2-F6AB4B814569}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+      <selection activeCell="L1" sqref="L1:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1631,11 +1631,11 @@
         <v>46.3</v>
       </c>
     </row>
-    <row r="33" spans="11:12" x14ac:dyDescent="0.2">
-      <c r="K33" t="s">
+    <row r="33" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L33" t="s">
         <v>30</v>
       </c>
-      <c r="L33">
+      <c r="M33">
         <f>AVERAGE(L1:L29)</f>
         <v>52.048275862068962</v>
       </c>
@@ -1647,10 +1647,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F16587F-151E-F944-A7AD-47F9A723EED8}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K29"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1658,7 +1658,7 @@
     <col min="1" max="1" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1692,8 +1692,12 @@
       <c r="K1">
         <v>838</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1">
+        <f>AVERAGE(B1:K1)</f>
+        <v>982.2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1727,8 +1731,12 @@
       <c r="K2">
         <v>907</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2">
+        <f t="shared" ref="L2:L29" si="0">AVERAGE(B2:K2)</f>
+        <v>1126.5999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1762,8 +1770,12 @@
       <c r="K3">
         <v>597</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>1069.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1797,8 +1809,12 @@
       <c r="K4">
         <v>1531</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1832,8 +1848,12 @@
       <c r="K5">
         <v>903</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1867,8 +1887,12 @@
       <c r="K6">
         <v>912</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1902,8 +1926,12 @@
       <c r="K7">
         <v>909</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>1205.4000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1937,8 +1965,12 @@
       <c r="K8">
         <v>2199</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>1420.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1972,8 +2004,12 @@
       <c r="K9">
         <v>1565</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>1258.9000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2007,8 +2043,12 @@
       <c r="K10">
         <v>1536</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>1354.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2042,8 +2082,12 @@
       <c r="K11">
         <v>1520</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>1349.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2077,8 +2121,12 @@
       <c r="K12">
         <v>1551</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>1356.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2112,8 +2160,12 @@
       <c r="K13">
         <v>1552</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2147,8 +2199,12 @@
       <c r="K14">
         <v>1549</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>1233.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2182,8 +2238,12 @@
       <c r="K15">
         <v>1516</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>1376.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2217,8 +2277,12 @@
       <c r="K16">
         <v>1563</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>1385.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2252,8 +2316,12 @@
       <c r="K17">
         <v>1535</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>1470.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2287,8 +2355,12 @@
       <c r="K18">
         <v>1546</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>1359.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2322,8 +2394,12 @@
       <c r="K19">
         <v>1526</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>1329.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2357,8 +2433,12 @@
       <c r="K20">
         <v>929</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>1330.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2392,8 +2472,12 @@
       <c r="K21">
         <v>1209</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>1224.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2427,8 +2511,12 @@
       <c r="K22">
         <v>1560</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>1197.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2462,8 +2550,12 @@
       <c r="K23">
         <v>584</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>1130.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2497,8 +2589,12 @@
       <c r="K24">
         <v>1205</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>1414.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2532,8 +2628,12 @@
       <c r="K25">
         <v>900</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>1257.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2567,8 +2667,12 @@
       <c r="K26">
         <v>1210</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>1316.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2602,8 +2706,12 @@
       <c r="K27">
         <v>1847</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>1447.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2637,8 +2745,12 @@
       <c r="K28">
         <v>1536</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>1326.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2671,6 +2783,19 @@
       </c>
       <c r="K29">
         <v>1531</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>1287.5999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L33" t="s">
+        <v>30</v>
+      </c>
+      <c r="M33">
+        <f>AVERAGE(L1:L29)</f>
+        <v>1299.6793103448272</v>
       </c>
     </row>
   </sheetData>
@@ -2680,10 +2805,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE50FE21-6C3F-A64C-8473-A905EC1E2CAA}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3315,7 +3440,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -3354,7 +3479,7 @@
         <v>82.2</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -3393,7 +3518,7 @@
         <v>83.3</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -3432,7 +3557,7 @@
         <v>81.3</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -3471,7 +3596,7 @@
         <v>106.6</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -3510,7 +3635,7 @@
         <v>96.7</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -3549,7 +3674,7 @@
         <v>91.8</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -3588,7 +3713,7 @@
         <v>90.2</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -3627,7 +3752,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -3666,7 +3791,7 @@
         <v>104.9</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -3705,7 +3830,7 @@
         <v>108.2</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -3744,7 +3869,7 @@
         <v>102.7</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -3783,7 +3908,7 @@
         <v>103.9</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -3822,11 +3947,11 @@
         <v>102.4</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K31" t="s">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L31" t="s">
         <v>29</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <f>AVERAGE(L1:L29)</f>
         <v>96.93793103448273</v>
       </c>
@@ -4996,10 +5121,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51C71A4E-2FDF-EA4C-9AAD-01142FD19753}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K29"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5007,7 +5132,7 @@
     <col min="1" max="1" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5041,8 +5166,12 @@
       <c r="K1">
         <v>324</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1">
+        <f>AVERAGE(B1:K1)</f>
+        <v>215.3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5076,8 +5205,12 @@
       <c r="K2">
         <v>248</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2">
+        <f t="shared" ref="L2:L29" si="0">AVERAGE(B2:K2)</f>
+        <v>219.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -5111,8 +5244,12 @@
       <c r="K3">
         <v>249</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>171.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5146,8 +5283,12 @@
       <c r="K4">
         <v>250</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>218.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -5181,8 +5322,12 @@
       <c r="K5">
         <v>247</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>212.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -5216,8 +5361,12 @@
       <c r="K6">
         <v>130</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>233.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -5251,8 +5400,12 @@
       <c r="K7">
         <v>126</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>205.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -5286,8 +5439,12 @@
       <c r="K8">
         <v>300</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>245.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -5321,8 +5478,12 @@
       <c r="K9">
         <v>386</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>217.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -5356,8 +5517,12 @@
       <c r="K10">
         <v>137</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>169.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -5391,8 +5556,12 @@
       <c r="K11">
         <v>246</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>219.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -5426,8 +5595,12 @@
       <c r="K12">
         <v>131</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>257.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -5461,8 +5634,12 @@
       <c r="K13">
         <v>133</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>226.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -5496,8 +5673,12 @@
       <c r="K14">
         <v>244</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -5531,8 +5712,12 @@
       <c r="K15">
         <v>250</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>252.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -5566,8 +5751,12 @@
       <c r="K16">
         <v>247</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>157.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -5601,8 +5790,12 @@
       <c r="K17">
         <v>418</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>236.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -5636,8 +5829,12 @@
       <c r="K18">
         <v>236</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>200.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -5671,8 +5868,12 @@
       <c r="K19">
         <v>136</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>256.39999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -5706,8 +5907,12 @@
       <c r="K20">
         <v>249</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>242.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -5741,8 +5946,12 @@
       <c r="K21">
         <v>138</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>203.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -5776,8 +5985,12 @@
       <c r="K22">
         <v>241</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>216.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -5811,8 +6024,12 @@
       <c r="K23">
         <v>253</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>218.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -5846,8 +6063,12 @@
       <c r="K24">
         <v>240</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>206.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -5881,8 +6102,12 @@
       <c r="K25">
         <v>138</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>239.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -5916,8 +6141,12 @@
       <c r="K26">
         <v>138</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>214.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -5951,8 +6180,12 @@
       <c r="K27">
         <v>267</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>280.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -5986,8 +6219,12 @@
       <c r="K28">
         <v>248</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -6020,6 +6257,19 @@
       </c>
       <c r="K29">
         <v>242</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>195.2</v>
+      </c>
+    </row>
+    <row r="33" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L33" t="s">
+        <v>30</v>
+      </c>
+      <c r="M33">
+        <f>AVERAGE(L1:L29)</f>
+        <v>221.35517241379307</v>
       </c>
     </row>
   </sheetData>
@@ -6029,10 +6279,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D632CAF-DA25-0244-9C87-308643069665}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K29"/>
+      <selection activeCell="L1" sqref="L1:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6040,7 +6290,7 @@
     <col min="1" max="1" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6074,8 +6324,12 @@
       <c r="K1">
         <v>408</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1">
+        <f>AVERAGE(B1:K1)</f>
+        <v>244.1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6109,8 +6363,12 @@
       <c r="K2">
         <v>470</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2">
+        <f t="shared" ref="L2:L29" si="0">AVERAGE(B2:K2)</f>
+        <v>345.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6144,8 +6402,12 @@
       <c r="K3">
         <v>311</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -6179,8 +6441,12 @@
       <c r="K4">
         <v>167</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>296.60000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -6214,8 +6480,12 @@
       <c r="K5">
         <v>168</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>300.89999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -6249,8 +6519,12 @@
       <c r="K6">
         <v>308</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>314.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -6284,8 +6558,12 @@
       <c r="K7">
         <v>291</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>323.89999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -6319,8 +6597,12 @@
       <c r="K8">
         <v>355</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>322.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -6354,8 +6636,12 @@
       <c r="K9">
         <v>457</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>386.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -6389,8 +6675,12 @@
       <c r="K10">
         <v>468</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>294.10000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -6424,8 +6714,12 @@
       <c r="K11">
         <v>465</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>345.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -6459,8 +6753,12 @@
       <c r="K12">
         <v>303</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>294.39999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -6494,8 +6792,12 @@
       <c r="K13">
         <v>166</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>300.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -6529,8 +6831,12 @@
       <c r="K14">
         <v>168</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>332.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -6564,8 +6870,12 @@
       <c r="K15">
         <v>298</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>312.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -6599,8 +6909,12 @@
       <c r="K16">
         <v>292</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>336.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -6634,8 +6948,12 @@
       <c r="K17">
         <v>302</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>315.39999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -6669,8 +6987,12 @@
       <c r="K18">
         <v>479</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>270.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -6704,8 +7026,12 @@
       <c r="K19">
         <v>472</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>347.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -6739,8 +7065,12 @@
       <c r="K20">
         <v>483</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>377.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -6774,8 +7104,12 @@
       <c r="K21">
         <v>297</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>341</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -6809,8 +7143,12 @@
       <c r="K22">
         <v>172</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>272.10000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -6844,8 +7182,12 @@
       <c r="K23">
         <v>161</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>313.60000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -6879,8 +7221,12 @@
       <c r="K24">
         <v>289</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>296.60000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -6914,8 +7260,12 @@
       <c r="K25">
         <v>298</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>338.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -6949,8 +7299,12 @@
       <c r="K26">
         <v>306</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>301.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -6984,8 +7338,12 @@
       <c r="K27">
         <v>459</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>296.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -7019,8 +7377,12 @@
       <c r="K28">
         <v>493</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>301.89999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -7053,6 +7415,19 @@
       </c>
       <c r="K29">
         <v>486</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>329.4</v>
+      </c>
+    </row>
+    <row r="33" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L33" t="s">
+        <v>30</v>
+      </c>
+      <c r="M33">
+        <f>AVERAGE(L1:L29)</f>
+        <v>316.69655172413798</v>
       </c>
     </row>
   </sheetData>
@@ -7062,10 +7437,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{505DA02D-D3C3-1B44-8C93-8D1DF543648E}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K29"/>
+      <selection activeCell="L1" sqref="L1:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7073,7 +7448,7 @@
     <col min="1" max="1" width="40.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7107,8 +7482,12 @@
       <c r="K1">
         <v>201</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1">
+        <f>AVERAGE(B1:K1)</f>
+        <v>216.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -7142,8 +7521,12 @@
       <c r="K2">
         <v>370</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2">
+        <f t="shared" ref="L2:L29" si="0">AVERAGE(B2:K2)</f>
+        <v>404.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -7177,8 +7560,12 @@
       <c r="K3">
         <v>360</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -7212,8 +7599,12 @@
       <c r="K4">
         <v>363</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>351.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -7247,8 +7638,12 @@
       <c r="K5">
         <v>365</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>359.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -7282,8 +7677,12 @@
       <c r="K6">
         <v>369</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>459.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -7317,8 +7716,12 @@
       <c r="K7">
         <v>364</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>478.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -7352,8 +7755,12 @@
       <c r="K8">
         <v>371</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>452</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -7387,8 +7794,12 @@
       <c r="K9">
         <v>555</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>444.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -7422,8 +7833,12 @@
       <c r="K10">
         <v>364</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>367.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -7457,8 +7872,12 @@
       <c r="K11">
         <v>373</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>401.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -7492,8 +7911,12 @@
       <c r="K12">
         <v>372</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>381</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -7527,8 +7950,12 @@
       <c r="K13">
         <v>363</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>383.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -7562,8 +7989,12 @@
       <c r="K14">
         <v>378</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>391.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -7597,8 +8028,12 @@
       <c r="K15">
         <v>355</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>443.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -7632,8 +8067,12 @@
       <c r="K16">
         <v>367</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>398.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -7667,8 +8106,12 @@
       <c r="K17">
         <v>557</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>438.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -7702,8 +8145,12 @@
       <c r="K18">
         <v>379</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>381</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -7737,8 +8184,12 @@
       <c r="K19">
         <v>366</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>405.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -7772,8 +8223,12 @@
       <c r="K20">
         <v>361</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>475.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -7807,8 +8262,12 @@
       <c r="K21">
         <v>410</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>367.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -7842,8 +8301,12 @@
       <c r="K22">
         <v>366</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>480.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -7877,8 +8340,12 @@
       <c r="K23">
         <v>381</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>423</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -7912,8 +8379,12 @@
       <c r="K24">
         <v>375</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>401.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -7947,8 +8418,12 @@
       <c r="K25">
         <v>595</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>408.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -7982,8 +8457,12 @@
       <c r="K26">
         <v>358</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>383.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -8017,8 +8496,12 @@
       <c r="K27">
         <v>364</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>424.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -8052,8 +8535,12 @@
       <c r="K28">
         <v>379</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>403.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -8086,6 +8573,19 @@
       </c>
       <c r="K29">
         <v>376</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>458.2</v>
+      </c>
+    </row>
+    <row r="33" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L33" t="s">
+        <v>30</v>
+      </c>
+      <c r="M33">
+        <f>AVERAGE(L1:L29)</f>
+        <v>405.72068965517246</v>
       </c>
     </row>
   </sheetData>
@@ -8095,10 +8595,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4EDAC9-16F9-2C4E-9FCF-1C37EF3AAF9D}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K29"/>
+      <selection activeCell="L1" sqref="L1:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8106,7 +8606,7 @@
     <col min="1" max="1" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8140,8 +8640,12 @@
       <c r="K1">
         <v>427</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1">
+        <f>AVERAGE(B1:K1)</f>
+        <v>382.3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -8175,8 +8679,12 @@
       <c r="K2">
         <v>655</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2">
+        <f t="shared" ref="L2:L29" si="0">AVERAGE(B2:K2)</f>
+        <v>492.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -8210,8 +8718,12 @@
       <c r="K3">
         <v>643</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>589.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -8245,8 +8757,12 @@
       <c r="K4">
         <v>419</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>494.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -8280,8 +8796,12 @@
       <c r="K5">
         <v>636</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>574.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -8315,8 +8835,12 @@
       <c r="K6">
         <v>228</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>543.29999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -8350,8 +8874,12 @@
       <c r="K7">
         <v>649</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>601.79999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -8385,8 +8913,12 @@
       <c r="K8">
         <v>671</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>593.70000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -8420,8 +8952,12 @@
       <c r="K9">
         <v>639</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>556.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -8455,8 +8991,12 @@
       <c r="K10">
         <v>427</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>514.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -8490,8 +9030,12 @@
       <c r="K11">
         <v>660</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>541.79999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -8525,8 +9069,12 @@
       <c r="K12">
         <v>641</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>538.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -8560,8 +9108,12 @@
       <c r="K13">
         <v>649</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>557.70000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -8595,8 +9147,12 @@
       <c r="K14">
         <v>668</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>717.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -8630,8 +9186,12 @@
       <c r="K15">
         <v>686</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>627.29999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -8665,8 +9225,12 @@
       <c r="K16">
         <v>654</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>536.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -8700,8 +9264,12 @@
       <c r="K17">
         <v>225</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>517.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -8735,8 +9303,12 @@
       <c r="K18">
         <v>430</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>556.79999999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -8770,8 +9342,12 @@
       <c r="K19">
         <v>422</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>557.79999999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -8805,8 +9381,12 @@
       <c r="K20">
         <v>431</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>614.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -8840,8 +9420,12 @@
       <c r="K21">
         <v>433</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>588</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -8875,8 +9459,12 @@
       <c r="K22">
         <v>656</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>535.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -8910,8 +9498,12 @@
       <c r="K23">
         <v>642</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>582</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -8945,8 +9537,12 @@
       <c r="K24">
         <v>646</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>538.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -8980,8 +9576,12 @@
       <c r="K25">
         <v>428</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>497.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -9015,8 +9615,12 @@
       <c r="K26">
         <v>414</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>643.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -9050,8 +9654,12 @@
       <c r="K27">
         <v>432</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>614.79999999999995</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -9085,8 +9693,12 @@
       <c r="K28">
         <v>652</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>694.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -9119,6 +9731,19 @@
       </c>
       <c r="K29">
         <v>900</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>672.1</v>
+      </c>
+    </row>
+    <row r="33" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L33" t="s">
+        <v>30</v>
+      </c>
+      <c r="M33">
+        <f>AVERAGE(L1:L29)</f>
+        <v>568.1241379310344</v>
       </c>
     </row>
   </sheetData>
@@ -9128,10 +9753,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB3BBBE-0EEA-9F43-94C6-20367BFA16DE}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K30"/>
+      <selection activeCell="L1" sqref="L1:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9139,7 +9764,7 @@
     <col min="1" max="1" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9173,8 +9798,12 @@
       <c r="K1">
         <v>747</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1">
+        <f>AVERAGE(B1:K1)</f>
+        <v>459.2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -9208,8 +9837,12 @@
       <c r="K2">
         <v>755</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2">
+        <f t="shared" ref="L2:L29" si="0">AVERAGE(B2:K2)</f>
+        <v>733.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -9243,8 +9876,12 @@
       <c r="K3">
         <v>978</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>761.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -9278,8 +9915,12 @@
       <c r="K4">
         <v>995</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>864.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -9313,8 +9954,12 @@
       <c r="K5">
         <v>1002</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>1015.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -9348,8 +9993,12 @@
       <c r="K6">
         <v>738</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>887</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -9383,8 +10032,12 @@
       <c r="K7">
         <v>992</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>813.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -9418,8 +10071,12 @@
       <c r="K8">
         <v>1018</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>838.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -9453,8 +10110,12 @@
       <c r="K9">
         <v>1011</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>969.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -9488,8 +10149,12 @@
       <c r="K10">
         <v>730</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>912.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -9523,8 +10188,12 @@
       <c r="K11">
         <v>996</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>861.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -9558,8 +10227,12 @@
       <c r="K12">
         <v>1002</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>789.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -9593,8 +10266,12 @@
       <c r="K13">
         <v>1016</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>900.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -9628,8 +10305,12 @@
       <c r="K14">
         <v>742</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>965.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -9663,8 +10344,12 @@
       <c r="K15">
         <v>987</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>916.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -9698,8 +10383,12 @@
       <c r="K16">
         <v>977</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>819.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -9733,8 +10422,12 @@
       <c r="K17">
         <v>1000</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>893.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -9768,8 +10461,12 @@
       <c r="K18">
         <v>738</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>919.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -9803,8 +10500,12 @@
       <c r="K19">
         <v>973</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>969.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -9838,8 +10539,12 @@
       <c r="K20">
         <v>987</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>856.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -9873,8 +10578,12 @@
       <c r="K21">
         <v>988</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>862.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -9908,8 +10617,12 @@
       <c r="K22">
         <v>728</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>891.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -9943,8 +10656,12 @@
       <c r="K23">
         <v>997</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>967.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -9978,8 +10695,12 @@
       <c r="K24">
         <v>991</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>893</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -10013,8 +10734,12 @@
       <c r="K25">
         <v>970</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>888.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -10048,8 +10773,12 @@
       <c r="K26">
         <v>726</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>841</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -10083,8 +10812,12 @@
       <c r="K27">
         <v>991</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>888.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -10118,8 +10851,12 @@
       <c r="K28">
         <v>975</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>832.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -10152,6 +10889,19 @@
       </c>
       <c r="K29">
         <v>988</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>948</v>
+      </c>
+    </row>
+    <row r="33" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L33" t="s">
+        <v>30</v>
+      </c>
+      <c r="M33">
+        <f>AVERAGE(L1:L29)</f>
+        <v>867.56206896551714</v>
       </c>
     </row>
   </sheetData>
@@ -10161,10 +10911,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{887663EF-40C0-424B-B2B6-EE04940D72D5}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K29"/>
+      <selection activeCell="L1" sqref="L1:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10172,7 +10922,7 @@
     <col min="1" max="1" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10206,8 +10956,12 @@
       <c r="K1">
         <v>496</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1">
+        <f>AVERAGE(B1:K1)</f>
+        <v>538.6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -10241,8 +10995,12 @@
       <c r="K2">
         <v>525</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2">
+        <f t="shared" ref="L2:L29" si="0">AVERAGE(B2:K2)</f>
+        <v>683.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -10276,8 +11034,12 @@
       <c r="K3">
         <v>532</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>856.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -10311,8 +11073,12 @@
       <c r="K4">
         <v>833</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>879.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -10346,8 +11112,12 @@
       <c r="K5">
         <v>1398</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>1055.0999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -10381,8 +11151,12 @@
       <c r="K6">
         <v>544</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>1023.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -10416,8 +11190,12 @@
       <c r="K7">
         <v>1136</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>856.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -10451,8 +11229,12 @@
       <c r="K8">
         <v>865</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>854.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -10486,8 +11268,12 @@
       <c r="K9">
         <v>818</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>737.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -10521,8 +11307,12 @@
       <c r="K10">
         <v>1115</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>999.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -10556,8 +11346,12 @@
       <c r="K11">
         <v>537</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>905.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -10591,8 +11385,12 @@
       <c r="K12">
         <v>1114</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>939.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -10626,8 +11424,12 @@
       <c r="K13">
         <v>539</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>854</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -10661,8 +11463,12 @@
       <c r="K14">
         <v>1382</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>1017.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -10696,8 +11502,12 @@
       <c r="K15">
         <v>829</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>974.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -10731,8 +11541,12 @@
       <c r="K16">
         <v>540</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>939.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -10766,8 +11580,12 @@
       <c r="K17">
         <v>1104</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>996.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -10801,8 +11619,12 @@
       <c r="K18">
         <v>860</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>943.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -10836,8 +11658,12 @@
       <c r="K19">
         <v>1107</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>995.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -10871,8 +11697,12 @@
       <c r="K20">
         <v>811</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>1041.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -10906,8 +11736,12 @@
       <c r="K21">
         <v>535</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>964</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -10941,8 +11775,12 @@
       <c r="K22">
         <v>1121</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>1015.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -10976,8 +11814,12 @@
       <c r="K23">
         <v>845</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>1031.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -11011,8 +11853,12 @@
       <c r="K24">
         <v>1087</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>990.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -11046,8 +11892,12 @@
       <c r="K25">
         <v>820</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>1081.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -11081,8 +11931,12 @@
       <c r="K26">
         <v>534</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>1001.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -11116,8 +11970,12 @@
       <c r="K27">
         <v>1113</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>994</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -11151,8 +12009,12 @@
       <c r="K28">
         <v>833</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>995.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -11185,6 +12047,19 @@
       </c>
       <c r="K29">
         <v>1105</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>1170.5</v>
+      </c>
+    </row>
+    <row r="33" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L33" t="s">
+        <v>30</v>
+      </c>
+      <c r="M33">
+        <f>AVERAGE(L1:L29)</f>
+        <v>942.56551724137944</v>
       </c>
     </row>
   </sheetData>

</xml_diff>